<commit_message>
XJDF-1262 Revised media size appendix to remove ancient cruft. Include new table to US Paper sizes.
</commit_message>
<xml_diff>
--- a/readme/Media Size Chart.xlsx
+++ b/readme/Media Size Chart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="127">
   <si>
     <t>1297 × 917</t>
   </si>
@@ -367,6 +367,36 @@
   </si>
   <si>
     <t>2.2 × 3.6</t>
+  </si>
+  <si>
+    <t>5.5 x 8.5</t>
+  </si>
+  <si>
+    <t>8.5 x 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.5 x 14 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.0 x 8.0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.0 x 17.0 </t>
+  </si>
+  <si>
+    <t>HalfLetter</t>
+  </si>
+  <si>
+    <t>Letter</t>
+  </si>
+  <si>
+    <t>Legal</t>
+  </si>
+  <si>
+    <t>JuniorLegal</t>
+  </si>
+  <si>
+    <t>LedgerTabloid</t>
   </si>
 </sst>
 </file>
@@ -374,7 +404,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -425,7 +455,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -721,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:Q60"/>
+  <dimension ref="A3:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="J68" sqref="J68"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J63" sqref="J63:K67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1566,7 +1596,7 @@
         <v>216</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" ref="E29:E33" si="15">RIGHT(B29,LEN(B29) - FIND("×",B29) -1)</f>
+        <f t="shared" ref="E29:E32" si="15">RIGHT(B29,LEN(B29) - FIND("×",B29) -1)</f>
         <v>279</v>
       </c>
       <c r="F29" t="str">
@@ -1665,7 +1695,7 @@
         <v>791</v>
       </c>
       <c r="M30">
-        <f t="shared" ref="M30:M33" si="31">ROUND(E30*$B$13, 0)</f>
+        <f t="shared" ref="M30:M32" si="31">ROUND(E30*$B$13, 0)</f>
         <v>1225</v>
       </c>
       <c r="N30" s="2">
@@ -1673,7 +1703,7 @@
         <v>792</v>
       </c>
       <c r="O30" s="2">
-        <f t="shared" ref="O30:O33" si="33">ROUND(G30*$C$13, 0)</f>
+        <f t="shared" ref="O30:O32" si="33">ROUND(G30*$C$13, 0)</f>
         <v>1224</v>
       </c>
       <c r="P30">
@@ -3291,6 +3321,286 @@
       <c r="Q60">
         <f t="shared" si="77"/>
         <v>-1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17">
+      <c r="A63" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63" t="s">
+        <v>117</v>
+      </c>
+      <c r="F63" t="str">
+        <f>LEFT(C63,FIND("x",C63)-2)</f>
+        <v>5.5</v>
+      </c>
+      <c r="G63" t="str">
+        <f>RIGHT(C63,LEN(C63) - FIND("x",C63) -1)</f>
+        <v>8.5</v>
+      </c>
+      <c r="H63" s="4">
+        <f t="shared" ref="H63:H67" si="78">ROUND(D63/$H$13,1)</f>
+        <v>0</v>
+      </c>
+      <c r="I63" s="4">
+        <f t="shared" ref="I63:I67" si="79">ROUND(E63/$H$13,1)</f>
+        <v>0</v>
+      </c>
+      <c r="J63" s="4">
+        <f t="shared" ref="J63:J67" si="80">ROUND(F63*$H$13,1)</f>
+        <v>139.69999999999999</v>
+      </c>
+      <c r="K63" s="4">
+        <f t="shared" ref="K63:K67" si="81">ROUND(G63*$H$13,1)</f>
+        <v>215.9</v>
+      </c>
+      <c r="L63" s="2">
+        <f t="shared" ref="L63:L67" si="82">ROUND(D63*$B$13, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M63" s="2">
+        <f t="shared" ref="M63:M67" si="83">ROUND(E63*$B$13, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N63">
+        <f t="shared" ref="N63:N67" si="84">ROUND(F63*$C$13, 0)</f>
+        <v>396</v>
+      </c>
+      <c r="O63">
+        <f t="shared" ref="O63:O67" si="85">ROUND(G63*$C$13, 0)</f>
+        <v>612</v>
+      </c>
+      <c r="P63">
+        <f t="shared" ref="P63:P67" si="86">L63-N63</f>
+        <v>-396</v>
+      </c>
+      <c r="Q63">
+        <f t="shared" ref="Q63:Q67" si="87">M63-O63</f>
+        <v>-612</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17">
+      <c r="A64" t="s">
+        <v>123</v>
+      </c>
+      <c r="C64" t="s">
+        <v>118</v>
+      </c>
+      <c r="F64" t="str">
+        <f t="shared" ref="F64:F67" si="88">LEFT(C64,FIND("x",C64)-2)</f>
+        <v>8.5</v>
+      </c>
+      <c r="G64" t="str">
+        <f t="shared" ref="G64:G67" si="89">RIGHT(C64,LEN(C64) - FIND("x",C64) -1)</f>
+        <v>11</v>
+      </c>
+      <c r="H64" s="4">
+        <f t="shared" si="78"/>
+        <v>0</v>
+      </c>
+      <c r="I64" s="4">
+        <f t="shared" si="79"/>
+        <v>0</v>
+      </c>
+      <c r="J64" s="4">
+        <f t="shared" si="80"/>
+        <v>215.9</v>
+      </c>
+      <c r="K64" s="4">
+        <f t="shared" si="81"/>
+        <v>279.39999999999998</v>
+      </c>
+      <c r="L64" s="2">
+        <f t="shared" si="82"/>
+        <v>0</v>
+      </c>
+      <c r="M64" s="2">
+        <f t="shared" si="83"/>
+        <v>0</v>
+      </c>
+      <c r="N64">
+        <f t="shared" si="84"/>
+        <v>612</v>
+      </c>
+      <c r="O64">
+        <f t="shared" si="85"/>
+        <v>792</v>
+      </c>
+      <c r="P64">
+        <f t="shared" si="86"/>
+        <v>-612</v>
+      </c>
+      <c r="Q64">
+        <f t="shared" si="87"/>
+        <v>-792</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17">
+      <c r="A65" t="s">
+        <v>124</v>
+      </c>
+      <c r="C65" t="s">
+        <v>119</v>
+      </c>
+      <c r="F65" t="str">
+        <f t="shared" si="88"/>
+        <v>8.5</v>
+      </c>
+      <c r="G65" t="str">
+        <f t="shared" si="89"/>
+        <v xml:space="preserve">14 </v>
+      </c>
+      <c r="H65" s="4">
+        <f t="shared" si="78"/>
+        <v>0</v>
+      </c>
+      <c r="I65" s="4">
+        <f t="shared" si="79"/>
+        <v>0</v>
+      </c>
+      <c r="J65" s="4">
+        <f t="shared" si="80"/>
+        <v>215.9</v>
+      </c>
+      <c r="K65" s="4">
+        <f t="shared" si="81"/>
+        <v>355.6</v>
+      </c>
+      <c r="L65" s="2">
+        <f t="shared" si="82"/>
+        <v>0</v>
+      </c>
+      <c r="M65" s="2">
+        <f t="shared" si="83"/>
+        <v>0</v>
+      </c>
+      <c r="N65">
+        <f t="shared" si="84"/>
+        <v>612</v>
+      </c>
+      <c r="O65">
+        <f t="shared" si="85"/>
+        <v>1008</v>
+      </c>
+      <c r="P65">
+        <f t="shared" si="86"/>
+        <v>-612</v>
+      </c>
+      <c r="Q65">
+        <f t="shared" si="87"/>
+        <v>-1008</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17">
+      <c r="A66" t="s">
+        <v>125</v>
+      </c>
+      <c r="C66" t="s">
+        <v>120</v>
+      </c>
+      <c r="F66" t="str">
+        <f t="shared" si="88"/>
+        <v>5.0</v>
+      </c>
+      <c r="G66" t="str">
+        <f t="shared" si="89"/>
+        <v xml:space="preserve">8.0 </v>
+      </c>
+      <c r="H66" s="4">
+        <f t="shared" si="78"/>
+        <v>0</v>
+      </c>
+      <c r="I66" s="4">
+        <f t="shared" si="79"/>
+        <v>0</v>
+      </c>
+      <c r="J66" s="4">
+        <f t="shared" si="80"/>
+        <v>127</v>
+      </c>
+      <c r="K66" s="4">
+        <f t="shared" si="81"/>
+        <v>203.2</v>
+      </c>
+      <c r="L66" s="2">
+        <f t="shared" si="82"/>
+        <v>0</v>
+      </c>
+      <c r="M66" s="2">
+        <f t="shared" si="83"/>
+        <v>0</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="84"/>
+        <v>360</v>
+      </c>
+      <c r="O66">
+        <f t="shared" si="85"/>
+        <v>576</v>
+      </c>
+      <c r="P66">
+        <f t="shared" si="86"/>
+        <v>-360</v>
+      </c>
+      <c r="Q66">
+        <f t="shared" si="87"/>
+        <v>-576</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17">
+      <c r="A67" t="s">
+        <v>126</v>
+      </c>
+      <c r="C67" t="s">
+        <v>121</v>
+      </c>
+      <c r="F67" t="str">
+        <f t="shared" si="88"/>
+        <v>11.0</v>
+      </c>
+      <c r="G67" t="str">
+        <f t="shared" si="89"/>
+        <v xml:space="preserve">17.0 </v>
+      </c>
+      <c r="H67" s="4">
+        <f t="shared" si="78"/>
+        <v>0</v>
+      </c>
+      <c r="I67" s="4">
+        <f t="shared" si="79"/>
+        <v>0</v>
+      </c>
+      <c r="J67" s="4">
+        <f t="shared" si="80"/>
+        <v>279.39999999999998</v>
+      </c>
+      <c r="K67" s="4">
+        <f t="shared" si="81"/>
+        <v>431.8</v>
+      </c>
+      <c r="L67" s="2">
+        <f t="shared" si="82"/>
+        <v>0</v>
+      </c>
+      <c r="M67" s="2">
+        <f t="shared" si="83"/>
+        <v>0</v>
+      </c>
+      <c r="N67">
+        <f t="shared" si="84"/>
+        <v>792</v>
+      </c>
+      <c r="O67">
+        <f t="shared" si="85"/>
+        <v>1224</v>
+      </c>
+      <c r="P67">
+        <f t="shared" si="86"/>
+        <v>-792</v>
+      </c>
+      <c r="Q67">
+        <f t="shared" si="87"/>
+        <v>-1224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>